<commit_message>
Export Plots as Images (in .fld dir)
</commit_message>
<xml_diff>
--- a/Matthew Data.xlsx
+++ b/Matthew Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew/Dropbox/Matthew/Documents/RBE 2002/RBE_2002-Team_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55B5F4B-58CB-1F4C-8D8E-664EB896B555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369DA6FB-7FE6-FA49-99A7-3EC9CBD48B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{BF9086FB-EEDA-7340-B38B-24D87DE37DE0}"/>
+    <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BF9086FB-EEDA-7340-B38B-24D87DE37DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Q2 - 100 Effort" sheetId="1" r:id="rId1"/>
@@ -34617,8 +34617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A9300E-46C4-2A4D-950D-E28FCA0356E1}">
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46677,8 +46677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987B675-B009-BA40-81ED-1A7AFE5872B7}">
   <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D60" workbookViewId="0">
-      <selection activeCell="V69" sqref="V69"/>
+    <sheetView topLeftCell="D60" workbookViewId="0">
+      <selection activeCell="W71" sqref="W71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Average and Standard Dev for Q2
</commit_message>
<xml_diff>
--- a/Matthew Data.xlsx
+++ b/Matthew Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew/Dropbox/Matthew/Documents/RBE 2002/RBE_2002-Team_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369DA6FB-7FE6-FA49-99A7-3EC9CBD48B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837E18FE-F676-A341-B221-67D309B4A270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BF9086FB-EEDA-7340-B38B-24D87DE37DE0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Right Error (m/s)</t>
+  </si>
+  <si>
+    <t>Left Speed</t>
+  </si>
+  <si>
+    <t>Right Speed</t>
+  </si>
+  <si>
+    <t>Ave:</t>
+  </si>
+  <si>
+    <t>St Dev:</t>
   </si>
 </sst>
 </file>
@@ -33509,16 +33521,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -34615,10 +34627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A9300E-46C4-2A4D-950D-E28FCA0356E1}">
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34627,7 +34639,7 @@
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -34637,8 +34649,14 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>335.98</v>
       </c>
@@ -34648,8 +34666,22 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(A2:A200)</f>
+        <v>305.34140703517551</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(B2:B200)</f>
+        <v>312.98603015075372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>122.17</v>
       </c>
@@ -34660,8 +34692,22 @@
         <f>C2+50</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <f>STDEV(A2:A200)</f>
+        <v>14.296751239007154</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <f>STDEV(B2:B200)</f>
+        <v>15.153799664167165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>247.4</v>
       </c>
@@ -34673,7 +34719,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>281</v>
       </c>
@@ -34685,7 +34731,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>293.22000000000003</v>
       </c>
@@ -34697,7 +34743,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>299.32</v>
       </c>
@@ -34709,7 +34755,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>302.38</v>
       </c>
@@ -34721,7 +34767,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>299.32</v>
       </c>
@@ -34733,7 +34779,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>305.43</v>
       </c>
@@ -34745,7 +34791,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>302.38</v>
       </c>
@@ -34757,7 +34803,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>305.43</v>
       </c>
@@ -34769,7 +34815,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>305.43</v>
       </c>
@@ -34781,7 +34827,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>299.32</v>
       </c>
@@ -34793,7 +34839,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>305.43</v>
       </c>
@@ -34805,7 +34851,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>308.49</v>
       </c>

</xml_diff>